<commit_message>
Werkblad toevoegen voor 08917
</commit_message>
<xml_diff>
--- a/voucher-export.xlsx
+++ b/voucher-export.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Frederik/Library/Mobile Documents/com~apple~CloudDocs/Sites/git-ob2c/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frederik/Library/Mobile Documents/com~apple~CloudDocs/Sites/git-ob2c/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2F2CF8-5709-DA46-80A0-A8CB04C59189}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940F9C2D-F907-9C45-A9D2-C9ECDD19334C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{0B9CA819-6430-064D-AB9E-0776AE783779}"/>
+    <workbookView xWindow="8680" yWindow="2400" windowWidth="25600" windowHeight="15540" xr2:uid="{0B9CA819-6430-064D-AB9E-0776AE783779}"/>
   </bookViews>
   <sheets>
     <sheet name="08899" sheetId="1" r:id="rId1"/>
     <sheet name="08900" sheetId="2" r:id="rId2"/>
+    <sheet name="08917" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'08899'!$A$1:$B$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'08900'!$A$1:$B$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'08917'!$A$1:$B$7</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
   <si>
     <t>Winkel</t>
   </si>
@@ -418,7 +420,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:B7" xr:uid="{D28F2188-C164-1B46-B108-97876DE586EA}">
-    <sortState ref="A2:B7">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B7">
       <sortCondition ref="A1:A7"/>
     </sortState>
   </autoFilter>
@@ -450,7 +452,39 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:B7" xr:uid="{B6C1E1A6-B7CB-0047-B6B8-C180E92C45D5}">
-    <sortState ref="A2:B13">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B13">
+      <sortCondition ref="A1:A13"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A850F277-E97E-2D44-A086-6748EEFE9A21}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B7" xr:uid="{B6C1E1A6-B7CB-0047-B6B8-C180E92C45D5}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B13">
       <sortCondition ref="A1:A13"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Nieuwe credit refs 08935 en 08936
+ toevoegen vervaldatum als parameter voor linken van vouchercode aan juiste credit ref
</commit_message>
<xml_diff>
--- a/voucher-export.xlsx
+++ b/voucher-export.xlsx
@@ -1,28 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frederik/Library/Mobile Documents/com~apple~CloudDocs/Sites/git-ob2c/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5EEF85-1BE2-E547-A64E-7EE687590715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0CDCF0-5F12-E546-963A-2426D3ACC907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8680" yWindow="2400" windowWidth="25600" windowHeight="15540" xr2:uid="{0B9CA819-6430-064D-AB9E-0776AE783779}"/>
+    <workbookView xWindow="3000" yWindow="1980" windowWidth="25600" windowHeight="15540" xr2:uid="{0B9CA819-6430-064D-AB9E-0776AE783779}"/>
   </bookViews>
   <sheets>
     <sheet name="08899" sheetId="1" r:id="rId1"/>
     <sheet name="08900" sheetId="2" r:id="rId2"/>
     <sheet name="08917" sheetId="3" r:id="rId3"/>
     <sheet name="08924" sheetId="4" r:id="rId4"/>
+    <sheet name="08935" sheetId="5" r:id="rId5"/>
+    <sheet name="08936" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'08899'!$A$1:$B$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'08900'!$A$1:$B$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'08917'!$A$1:$B$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'08924'!$A$1:$B$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'08935'!$A$1:$B$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'08936'!$A$1:$B$7</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="2">
   <si>
     <t>Winkel</t>
   </si>
@@ -524,4 +528,68 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C3DC0B8-E181-CF45-ABA2-07F466402B83}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B7" xr:uid="{D28F2188-C164-1B46-B108-97876DE586EA}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B7">
+      <sortCondition ref="A1:A7"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0195E8B6-828F-5A4B-B4EF-86D541E5F34F}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B7" xr:uid="{D28F2188-C164-1B46-B108-97876DE586EA}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B7">
+      <sortCondition ref="A1:A7"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>